<commit_message>
news note repeats handling
</commit_message>
<xml_diff>
--- a/na-service/src/test/resources/func/parser/source/real/CNN - Source.xlsx
+++ b/na-service/src/test/resources/func/parser/source/real/CNN - Source.xlsx
@@ -58,7 +58,7 @@
     <t>cd__headline-text:STARTS</t>
   </si>
   <si>
-    <t>cd__headline:EQUALS</t>
+    <t>a:HTML_TAG</t>
   </si>
   <si>
     <t>Africa</t>
@@ -484,12 +484,12 @@
       <name val="Menlo"/>
     </font>
     <font>
+      <sz val="13.0"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="13.0"/>
-      <color rgb="FF000000"/>
     </font>
     <font/>
   </fonts>
@@ -533,13 +533,13 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -861,7 +861,7 @@
       <c r="F3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="3"/>
@@ -933,7 +933,7 @@
       <c r="F5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="3"/>
@@ -1005,7 +1005,7 @@
       <c r="F7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="3"/>
@@ -1077,7 +1077,7 @@
       <c r="F9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="3"/>
@@ -1149,7 +1149,7 @@
       <c r="F11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="3"/>
@@ -1221,7 +1221,7 @@
       <c r="F13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="3"/>
@@ -1293,7 +1293,7 @@
       <c r="F15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="3"/>
@@ -1365,7 +1365,7 @@
       <c r="F17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H17" s="3"/>
@@ -1437,7 +1437,7 @@
       <c r="F19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="3"/>
@@ -1509,7 +1509,7 @@
       <c r="F21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H21" s="3"/>
@@ -1581,7 +1581,7 @@
       <c r="F23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="3"/>
@@ -1653,7 +1653,7 @@
       <c r="F25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H25" s="3"/>
@@ -1725,7 +1725,7 @@
       <c r="F27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H27" s="3"/>
@@ -1797,7 +1797,7 @@
       <c r="F29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H29" s="3"/>
@@ -1827,7 +1827,7 @@
       <c r="B30" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1869,7 +1869,7 @@
       <c r="F31" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H31" s="3"/>
@@ -1899,7 +1899,7 @@
       <c r="B32" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1941,7 +1941,7 @@
       <c r="F33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H33" s="3"/>
@@ -2013,7 +2013,7 @@
       <c r="F35" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H35" s="3"/>
@@ -2085,7 +2085,7 @@
       <c r="F37" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H37" s="3"/>
@@ -2115,7 +2115,7 @@
       <c r="B38" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="8" t="s">
         <v>65</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -2157,7 +2157,7 @@
       <c r="F39" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H39" s="3"/>
@@ -2229,7 +2229,7 @@
       <c r="F41" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H41" s="3"/>
@@ -2301,7 +2301,7 @@
       <c r="F43" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H43" s="3"/>
@@ -2373,7 +2373,7 @@
       <c r="F45" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G45" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H45" s="3"/>
@@ -2445,7 +2445,7 @@
       <c r="F47" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G47" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H47" s="3"/>
@@ -2517,7 +2517,7 @@
       <c r="F49" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G49" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H49" s="3"/>
@@ -2589,7 +2589,7 @@
       <c r="F51" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G51" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H51" s="3"/>
@@ -2661,7 +2661,7 @@
       <c r="F53" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="G53" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H53" s="3"/>
@@ -2733,7 +2733,7 @@
       <c r="F55" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G55" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H55" s="3"/>
@@ -2805,7 +2805,7 @@
       <c r="F57" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="G57" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H57" s="3"/>
@@ -2877,7 +2877,7 @@
       <c r="F59" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="G59" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H59" s="3"/>
@@ -3117,7 +3117,7 @@
       <c r="B66" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="8" t="s">
         <v>100</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -3369,7 +3369,7 @@
       <c r="F73" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G73" s="1" t="s">
+      <c r="G73" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H73" s="3"/>
@@ -3441,7 +3441,7 @@
       <c r="F75" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="G75" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H75" s="3"/>
@@ -3471,7 +3471,7 @@
       <c r="B76" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -3513,7 +3513,7 @@
       <c r="F77" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G77" s="1" t="s">
+      <c r="G77" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H77" s="3"/>
@@ -3585,7 +3585,7 @@
       <c r="F79" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G79" s="1" t="s">
+      <c r="G79" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H79" s="3"/>
@@ -3657,7 +3657,7 @@
       <c r="F81" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G81" s="1" t="s">
+      <c r="G81" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H81" s="3"/>
@@ -3687,7 +3687,7 @@
       <c r="B82" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="C82" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -3729,7 +3729,7 @@
       <c r="F83" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G83" s="1" t="s">
+      <c r="G83" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H83" s="3"/>
@@ -3801,7 +3801,7 @@
       <c r="F85" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G85" s="1" t="s">
+      <c r="G85" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H85" s="3"/>
@@ -3873,7 +3873,7 @@
       <c r="F87" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G87" s="1" t="s">
+      <c r="G87" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H87" s="3"/>
@@ -3945,7 +3945,7 @@
       <c r="F89" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G89" s="1" t="s">
+      <c r="G89" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H89" s="3"/>
@@ -4109,7 +4109,7 @@
       <c r="Z93" s="3"/>
     </row>
     <row r="94">
-      <c r="A94" s="8" t="s">
+      <c r="A94" s="7" t="s">
         <v>138</v>
       </c>
       <c r="B94" s="4" t="s">
@@ -4118,14 +4118,14 @@
       <c r="C94" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D94" s="8" t="s">
+      <c r="D94" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
-      <c r="I94" s="8" t="s">
+      <c r="I94" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J94" s="3"/>
@@ -4151,11 +4151,11 @@
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
-      <c r="E95" s="8" t="s">
+      <c r="E95" s="7" t="s">
         <v>134</v>
       </c>
       <c r="F95" s="9"/>
-      <c r="G95" s="8" t="s">
+      <c r="G95" s="7" t="s">
         <v>135</v>
       </c>
       <c r="H95" s="3"/>
@@ -4179,7 +4179,7 @@
       <c r="Z95" s="3"/>
     </row>
     <row r="96">
-      <c r="A96" s="8" t="s">
+      <c r="A96" s="7" t="s">
         <v>141</v>
       </c>
       <c r="B96" s="4" t="s">
@@ -4188,14 +4188,14 @@
       <c r="C96" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D96" s="8" t="s">
+      <c r="D96" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-      <c r="I96" s="8" t="s">
+      <c r="I96" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J96" s="3"/>
@@ -4227,7 +4227,7 @@
       <c r="F97" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G97" s="8" t="s">
+      <c r="G97" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H97" s="3"/>
@@ -4251,23 +4251,23 @@
       <c r="Z97" s="3"/>
     </row>
     <row r="98">
-      <c r="A98" s="8" t="s">
+      <c r="A98" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C98" s="8" t="s">
+      <c r="C98" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D98" s="8" t="s">
+      <c r="D98" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
-      <c r="I98" s="8" t="s">
+      <c r="I98" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J98" s="3"/>
@@ -4299,7 +4299,7 @@
       <c r="F99" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G99" s="8" t="s">
+      <c r="G99" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H99" s="3"/>

</xml_diff>